<commit_message>
adding pics and caps
</commit_message>
<xml_diff>
--- a/time_tracker.xlsx
+++ b/time_tracker.xlsx
@@ -137,6 +137,8 @@
     <sheet name="2025-07-28" sheetId="129" r:id="rId128"/>
     <sheet name="2025-07-29" sheetId="130" r:id="rId129"/>
     <sheet name="2025-07-30" sheetId="131" r:id="rId133"/>
+    <sheet name="2025-07-31" sheetId="132" r:id="rId134"/>
+    <sheet name="2025-08-01" sheetId="133" r:id="rId135"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -156,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5983" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="423">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1413,6 +1415,18 @@
   </si>
   <si>
     <t>212.0 minutes</t>
+  </si>
+  <si>
+    <t>87.0 minutes</t>
+  </si>
+  <si>
+    <t>1h in power outage</t>
+  </si>
+  <si>
+    <t>56.2 minutes</t>
+  </si>
+  <si>
+    <t>98.5 minutes</t>
   </si>
 </sst>
 </file>
@@ -7519,6 +7533,486 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>45868.029680444524</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>45868.029724235406</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>45868.029736617544</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>45868.68412563404</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>45868.693276289894</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>45868.69773115022</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>45868.79586219194</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>45868.79587357461</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>45868.83697349416</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>45868.84091909465</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>45868.96975878833</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>45868.97937125051</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet132.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>45869.13904485325</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>45869.16853983468</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>45869.17225669279</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>45869.17226873584</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>45869.69388996403</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>45869.706829199466</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>45869.706949185886</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>45869.73825937056</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>45869.75094358776</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>45869.7627205929</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>45869.7659765712</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>45869.766377614586</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>45869.7733095217</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>45869.77816754664</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>45869.77818606052</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>45869.78544918315</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>45869.85706285266</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>45869.924536419545</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>45869.94812862535</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>45869.94921022741</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>45869.9492358783</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
+        <v>45869.96214444255</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>45869.965250347675</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet133.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>45870.00046639558</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>45870.00047681589</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>45870.00048553194</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>

</xml_diff>